<commit_message>
fixed TJK summary page
</commit_message>
<xml_diff>
--- a/docs/Conduit_TJK_FP.xlsx
+++ b/docs/Conduit_TJK_FP.xlsx
@@ -553,36 +553,12 @@
     <t xml:space="preserve">Megjelenik a saját profilunk az aktuális adatokkal</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Módosítsuk a pofilunk adatait:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://www.gravatar.com/avatar/0?d=mp&amp;f=y
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Testuser11
+    <t xml:space="preserve">Módosítsuk a pofilunk adatait:
+https://www.gravatar.com/avatar/0?d=mp&amp;f=y
+Testuser11
 Testbio
 testuser11@gmail.com
 TestUser11</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Kattintsunk az Update Settngs gombra, majd az Ok gombra</t>
@@ -1022,7 +998,7 @@
     <cellStyle name="Normál 2" xfId="20"/>
     <cellStyle name="Excel_BuiltIn_Note" xfId="21"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="124">
     <dxf>
       <font>
         <name val="Sans"/>
@@ -1627,7 +1603,104 @@
       <font>
         <name val="Sans"/>
         <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
         <b val="0"/>
+        <i val="0"/>
         <color rgb="FF800080"/>
       </font>
       <fill>
@@ -1641,11 +1714,552 @@
         <name val="Sans"/>
         <family val="0"/>
         <b val="0"/>
+        <i val="0"/>
         <color rgb="FF008000"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1701,11 +2315,195 @@
       <font>
         <name val="Sans"/>
         <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
         <color rgb="FF800080"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Sans"/>
+        <family val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1785,15 +2583,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="47.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="47.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="60.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="60.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="5" style="1" width="11.25"/>
   </cols>
   <sheetData>
@@ -1977,7 +2775,7 @@
         <v>Pass</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1988,6 +2786,10 @@
         <f aca="false">CON_TC_013!J5</f>
         <v>Fail</v>
       </c>
+      <c r="D15" s="2" t="str">
+        <f aca="false">CON_TC_013!F25</f>
+        <v>A cikkhez tartozó tag-ek tartalma üres stringre változik</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
@@ -2025,7 +2827,7 @@
         <v>Pass</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>38</v>
       </c>
@@ -2036,6 +2838,10 @@
         <f aca="false">CON_TC_017!J5</f>
         <v>Fail</v>
       </c>
+      <c r="D19" s="2" t="str">
+        <f aca="false">CON_TC_017!F22</f>
+        <v>Üres lista jelenik meg</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
@@ -2049,7 +2855,7 @@
         <v>Pass</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
@@ -2060,8 +2866,12 @@
         <f aca="false">CON_TC_019!J5</f>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="2" t="str">
+        <f aca="false">CON_TC_019!F21</f>
+        <v>A szűrés nem működik, továbbra is az összes cikket kilistázza</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
@@ -2072,6 +2882,10 @@
         <f aca="false">CON_TC_020!J5</f>
         <v>Fail</v>
       </c>
+      <c r="D22" s="2" t="str">
+        <f aca="false">CON_TC_020!F21</f>
+        <v>A lista továbbra is az összes cikket tartalmazza</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
@@ -2085,7 +2899,7 @@
         <v>Pass</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -2095,6 +2909,10 @@
       <c r="C24" s="9" t="str">
         <f aca="false">CON_TC_022!J5</f>
         <v>Fail</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f aca="false">CON_TC_022!F23</f>
+        <v>Az email mező nem kerül frissítésre</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,14 +2966,14 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -2581,14 +3399,14 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="50.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="50.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -3033,10 +3851,10 @@
   </mergeCells>
   <conditionalFormatting sqref="I21:I22 I18:I19">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
@@ -3048,10 +3866,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3077,14 +3895,14 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -3557,18 +4375,18 @@
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="I21:I23 J5 I18:I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3594,14 +4412,14 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -4070,18 +4888,18 @@
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="I21:I23 J5 I18:I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4107,14 +4925,14 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -4529,18 +5347,18 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="I21 J5 I18:I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4566,14 +5384,14 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -5085,26 +5903,26 @@
     <mergeCell ref="I25:J25"/>
   </mergeCells>
   <conditionalFormatting sqref="I22:I24 I19:I20">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+      <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+      <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25 J5">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+      <formula>NOT(ISERROR(SEARCH("Fail",I25)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+      <formula>NOT(ISERROR(SEARCH("Pass",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5130,14 +5948,14 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -5612,18 +6430,18 @@
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="I21:I23 J5 I18:I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5649,14 +6467,14 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -6171,18 +6989,18 @@
     <mergeCell ref="I25:J25"/>
   </mergeCells>
   <conditionalFormatting sqref="I22:I25 J5 I19:I20">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+      <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6208,14 +7026,14 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -6720,18 +7538,18 @@
     <mergeCell ref="I25:J25"/>
   </mergeCells>
   <conditionalFormatting sqref="I23:I25 J5 I20:I21">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+      <formula>NOT(ISERROR(SEARCH("Fail",I23)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+      <formula>NOT(ISERROR(SEARCH("Pass",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
       <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6757,14 +7575,14 @@
       <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -7220,26 +8038,26 @@
     <mergeCell ref="I22:J22"/>
   </mergeCells>
   <conditionalFormatting sqref="I22 J5">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+      <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+      <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21 I18:I19">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7265,14 +8083,14 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -7644,14 +8462,14 @@
       <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -8078,26 +8896,26 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="I21 I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
-      <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
-      <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21 J5 I18:I19">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8119,18 +8937,18 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -8555,35 +9373,35 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
       <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
       <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I19">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
       <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21 J5">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8602,21 +9420,21 @@
     <tabColor rgb="FF008080"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="19.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="19.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="7" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="43.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="43.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -8995,8 +9813,6 @@
         <v>155</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="42">
     <mergeCell ref="A1:B1"/>
@@ -9043,34 +9859,34 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
       <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
       <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I19">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
       <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21 J5">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9096,14 +9912,14 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -9524,26 +10340,26 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="J5 I18:I19 I21">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+      <formula>NOT(ISERROR(SEARCH("Fail",J5)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+      <formula>NOT(ISERROR(SEARCH("Pass",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
       <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
       <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9565,18 +10381,18 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="75.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="75.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -9953,10 +10769,10 @@
       <c r="A22" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="26" t="s">
         <v>90</v>
       </c>
@@ -10049,39 +10865,39 @@
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="J5 I23">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
+      <formula>NOT(ISERROR(SEARCH("Fail",J5)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
+      <formula>NOT(ISERROR(SEARCH("Pass",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I19 I21:I22">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
       <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
       <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
       <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="https://www.gravatar.com/avatar/0?d=mp&amp;f=y"/>
+    <hyperlink ref="B22" r:id="rId1" display="Módosítsuk a pofilunk adatait:&#10;https://www.gravatar.com/avatar/0?d=mp&amp;f=y&#10;Testuser11&#10;Testbio&#10;testuser11@gmail.com&#10;TestUser11"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10105,14 +10921,14 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="25.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="25.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -10571,34 +11387,34 @@
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>NOT(ISERROR(SEARCH("Pass",J5)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
       <formula>NOT(ISERROR(SEARCH("Fail",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I20">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
       <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
       <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
       <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I23">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
       <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10624,14 +11440,14 @@
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -11042,14 +11858,14 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -11421,14 +12237,14 @@
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -11839,14 +12655,14 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="16.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="16.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -12232,14 +13048,14 @@
       <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -12665,14 +13481,14 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>
@@ -13104,14 +13920,14 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="12" style="10" width="8.87"/>
   </cols>
   <sheetData>

</xml_diff>